<commit_message>
fix summation, closes #2
</commit_message>
<xml_diff>
--- a/data-export/export_202110/sum_tagged_all_ops.xlsx
+++ b/data-export/export_202110/sum_tagged_all_ops.xlsx
@@ -429,25 +429,25 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>9945490156.799999</v>
+        <v>9934123224.118</v>
       </c>
       <c r="D2">
-        <v>58532633215.87</v>
+        <v>58468220597.456</v>
       </c>
       <c r="E2">
-        <v>68478123372.67</v>
+        <v>68402343821.574</v>
       </c>
       <c r="F2">
-        <v>3706247935.4</v>
+        <v>3702458957.841</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="I2">
-        <v>4309</v>
+        <v>4307.2</v>
       </c>
       <c r="J2">
         <v>39</v>
@@ -509,16 +509,16 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>9050548149.25</v>
+        <v>9048865628.261999</v>
       </c>
       <c r="D4">
-        <v>7633495812.41</v>
+        <v>7623961526.874</v>
       </c>
       <c r="E4">
-        <v>16684043961.66</v>
+        <v>16672827155.136</v>
       </c>
       <c r="F4">
-        <v>410094333.33</v>
+        <v>409533492.999</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -527,7 +527,7 @@
         <v>28</v>
       </c>
       <c r="I4">
-        <v>863</v>
+        <v>861.8</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -666,16 +666,16 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>6218982297.33</v>
+        <v>6182021288.07</v>
       </c>
       <c r="D8">
-        <v>35240899658.01</v>
+        <v>35031453945.68</v>
       </c>
       <c r="E8">
-        <v>41459881955.34</v>
+        <v>41213475233.75</v>
       </c>
       <c r="F8">
-        <v>78467742.69</v>
+        <v>66689341.37</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -706,13 +706,13 @@
         <v>0.4</v>
       </c>
       <c r="C9">
-        <v>8076536896.71</v>
+        <v>7738117045.82</v>
       </c>
       <c r="D9">
-        <v>44824244703.32</v>
+        <v>42906532215.63</v>
       </c>
       <c r="E9">
-        <v>52900781600.03</v>
+        <v>50644649261.45</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -786,13 +786,13 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>53076524038.24</v>
+        <v>40630694082.9138</v>
       </c>
       <c r="D11">
-        <v>38009533976.84</v>
+        <v>31157465121.36718</v>
       </c>
       <c r="E11">
-        <v>91087623958.31</v>
+        <v>71789725147.51099</v>
       </c>
       <c r="F11">
         <v>248264644.51</v>
@@ -810,10 +810,10 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>52829825336.96</v>
+        <v>40383995381.6338</v>
       </c>
       <c r="L11">
-        <v>-1.759469796525082e-07</v>
+        <v>-7.291299254580555e-08</v>
       </c>
     </row>
     <row r="12">
@@ -866,13 +866,13 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>12018683425.79</v>
+        <v>12014897623.82619</v>
       </c>
       <c r="D13">
-        <v>8462314705.75</v>
+        <v>8458455415.152819</v>
       </c>
       <c r="E13">
-        <v>20480998131.54</v>
+        <v>20473353038.97901</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -890,10 +890,10 @@
         <v>0</v>
       </c>
       <c r="K13">
-        <v>12018683425.79</v>
+        <v>12014897623.82619</v>
       </c>
       <c r="L13">
-        <v>-6.385016604326665e-08</v>
+        <v>-6.374381599011211e-08</v>
       </c>
     </row>
     <row r="14">
@@ -903,13 +903,13 @@
         </is>
       </c>
       <c r="C14">
-        <v>4644760.18</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>4620260.15</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>9265020.33</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -927,10 +927,10 @@
         <v>0</v>
       </c>
       <c r="K14">
-        <v>4644760.18</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <v>5.820766091346741e-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -943,13 +943,13 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>2059843919.05</v>
+        <v>1939791149.78</v>
       </c>
       <c r="D15">
-        <v>2059843911.04</v>
+        <v>1939791141.89</v>
       </c>
       <c r="E15">
-        <v>4119687830.09</v>
+        <v>3879582291.67</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>2515</v>
+        <v>2498</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -967,10 +967,10 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <v>303740299.72</v>
+        <v>301136639.18</v>
       </c>
       <c r="L15">
-        <v>959063604.48</v>
+        <v>952141088.34</v>
       </c>
     </row>
     <row r="16">
@@ -1063,16 +1063,16 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>718930567.85</v>
+        <v>711777908.9</v>
       </c>
       <c r="D18">
-        <v>4073939851.09</v>
+        <v>4033408119.89</v>
       </c>
       <c r="E18">
-        <v>4792870418.94</v>
+        <v>4745186028.79</v>
       </c>
       <c r="F18">
-        <v>718930567.85</v>
+        <v>711777908.9</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1103,34 +1103,34 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>14305621765.22</v>
+        <v>10545425542.81</v>
       </c>
       <c r="D19">
-        <v>62200397798.2</v>
+        <v>44640819939.96</v>
       </c>
       <c r="E19">
-        <v>76506019563.42</v>
+        <v>55186245482.77</v>
       </c>
       <c r="F19">
-        <v>11848430612.51</v>
+        <v>8510292862.8</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I19">
-        <v>1122</v>
+        <v>325</v>
       </c>
       <c r="J19">
-        <v>1382</v>
+        <v>1262</v>
       </c>
       <c r="K19">
-        <v>1608216850.72</v>
+        <v>1299514602.92</v>
       </c>
       <c r="L19">
-        <v>4236412054.16</v>
+        <v>3472373051.6</v>
       </c>
     </row>
     <row r="20">
@@ -1143,34 +1143,34 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>9537431329.809999</v>
+        <v>7833101837.679999</v>
       </c>
       <c r="D20">
-        <v>47256115447.62</v>
+        <v>37585148036.7</v>
       </c>
       <c r="E20">
-        <v>56793546777.43</v>
+        <v>45418249874.38</v>
       </c>
       <c r="F20">
-        <v>8019915133.21</v>
+        <v>6806868627.82</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>930</v>
+        <v>755</v>
       </c>
       <c r="I20">
-        <v>3815</v>
+        <v>2804</v>
       </c>
       <c r="J20">
-        <v>630</v>
+        <v>365</v>
       </c>
       <c r="K20">
-        <v>1004795438.29</v>
+        <v>586322949.54</v>
       </c>
       <c r="L20">
-        <v>155114706.77</v>
+        <v>95300561.51999998</v>
       </c>
     </row>
     <row r="21">
@@ -1183,13 +1183,13 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>4436062847.7</v>
+        <v>4421039742.67</v>
       </c>
       <c r="D21">
-        <v>21546195019.51</v>
+        <v>21492164851.48</v>
       </c>
       <c r="E21">
-        <v>25982257867.21</v>
+        <v>25913204594.15</v>
       </c>
       <c r="F21">
         <v>96769740.34</v>
@@ -1201,13 +1201,13 @@
         <v>22</v>
       </c>
       <c r="I21">
-        <v>5211</v>
+        <v>5204</v>
       </c>
       <c r="J21">
         <v>273</v>
       </c>
       <c r="K21">
-        <v>690245253.62</v>
+        <v>677721370.62</v>
       </c>
       <c r="L21">
         <v>-5.911715561524034e-09</v>

</xml_diff>

<commit_message>
update pages, also closes #8
</commit_message>
<xml_diff>
--- a/data-export/export_202110/sum_tagged_all_ops.xlsx
+++ b/data-export/export_202110/sum_tagged_all_ops.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -418,6 +418,11 @@
           <t>fin_vyuct_narodni_verejne</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>fin_vyuct_verejne</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -458,6 +463,9 @@
       <c r="L2">
         <v>481374754.2199999</v>
       </c>
+      <c r="M2">
+        <v>11553428901.86</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -498,6 +506,9 @@
       <c r="L3">
         <v>1013353.650000085</v>
       </c>
+      <c r="M3">
+        <v>7259831475.81</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -538,6 +549,9 @@
       <c r="L4">
         <v>2.863998815882951e-09</v>
       </c>
+      <c r="M4">
+        <v>3318112356.43</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -578,6 +592,9 @@
       <c r="L5">
         <v>0</v>
       </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -618,6 +635,9 @@
       <c r="L6">
         <v>0</v>
       </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -655,6 +675,9 @@
       <c r="L7">
         <v>0</v>
       </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -695,6 +718,9 @@
       <c r="L8">
         <v>0</v>
       </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -735,6 +761,9 @@
       <c r="L9">
         <v>-1.855369191616774e-09</v>
       </c>
+      <c r="M9">
+        <v>1706372594.94</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -775,6 +804,9 @@
       <c r="L10">
         <v>1.280568540096283e-09</v>
       </c>
+      <c r="M10">
+        <v>18561765.15</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -815,6 +847,9 @@
       <c r="L11">
         <v>-7.291299254580555e-08</v>
       </c>
+      <c r="M11">
+        <v>29750632143.26718</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -855,6 +890,9 @@
       <c r="L12">
         <v>4.270987119525671e-09</v>
       </c>
+      <c r="M12">
+        <v>637662428.21</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -893,7 +931,10 @@
         <v>12014897623.82619</v>
       </c>
       <c r="L13">
-        <v>-6.374381599011211e-08</v>
+        <v>-6.374381599011212e-08</v>
+      </c>
+      <c r="M13">
+        <v>8458455415.152819</v>
       </c>
     </row>
     <row r="14">
@@ -932,6 +973,9 @@
       <c r="L14">
         <v>0</v>
       </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -972,6 +1016,9 @@
       <c r="L15">
         <v>952141088.34</v>
       </c>
+      <c r="M15">
+        <v>2205418812.46</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1012,6 +1059,9 @@
       <c r="L16">
         <v>50607429.68</v>
       </c>
+      <c r="M16">
+        <v>113866716.77</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1052,6 +1102,9 @@
       <c r="L17">
         <v>323561093.41</v>
       </c>
+      <c r="M17">
+        <v>775373909.08</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1092,6 +1145,9 @@
       <c r="L18">
         <v>0</v>
       </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1132,6 +1188,9 @@
       <c r="L19">
         <v>3472373051.6</v>
       </c>
+      <c r="M19">
+        <v>23761275973.88</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1172,6 +1231,9 @@
       <c r="L20">
         <v>95300561.51999998</v>
       </c>
+      <c r="M20">
+        <v>3479432893.66</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1212,6 +1274,9 @@
       <c r="L21">
         <v>-5.911715561524034e-09</v>
       </c>
+      <c r="M21">
+        <v>2201763329.6</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1252,6 +1317,9 @@
       <c r="L22">
         <v>-3.275090421084315e-09</v>
       </c>
+      <c r="M22">
+        <v>2578418745.04</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1292,6 +1360,9 @@
       <c r="L23">
         <v>-1.280568540096283e-09</v>
       </c>
+      <c r="M23">
+        <v>67715138.94</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1332,6 +1403,9 @@
       <c r="L24">
         <v>0</v>
       </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1372,6 +1446,9 @@
       <c r="L25">
         <v>0</v>
       </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1410,6 +1487,9 @@
         <v>0</v>
       </c>
       <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "update data export"
This reverts commit 2f1369600ee5748f719a0ef78b19fe3287c9a686.
</commit_message>
<xml_diff>
--- a/data-export/export_202110/sum_tagged_all_ops.xlsx
+++ b/data-export/export_202110/sum_tagged_all_ops.xlsx
@@ -429,34 +429,34 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>11730842369.72506</v>
+        <v>11786696919.88891</v>
       </c>
       <c r="D2">
-        <v>68391315549.91532</v>
+        <v>68707778478.51116</v>
       </c>
       <c r="E2">
-        <v>80122157919.6404</v>
+        <v>80494475398.40007</v>
       </c>
       <c r="F2">
-        <v>141720819951.5819</v>
+        <v>141778049092.0393</v>
       </c>
       <c r="G2">
-        <v>122969771195.318</v>
+        <v>123040385205.7217</v>
       </c>
       <c r="H2">
-        <v>16556242699.06388</v>
+        <v>16587803787.86758</v>
       </c>
       <c r="I2">
-        <v>2194806057.2</v>
+        <v>2149860098.45</v>
       </c>
       <c r="J2">
-        <v>10172127247.12506</v>
+        <v>10227981797.28891</v>
       </c>
       <c r="K2">
-        <v>78563442797.04041</v>
+        <v>78935760275.80008</v>
       </c>
       <c r="L2">
-        <v>1558715122.600001</v>
+        <v>1558715122.6</v>
       </c>
     </row>
     <row r="3">
@@ -469,31 +469,31 @@
         <v>0.4</v>
       </c>
       <c r="C3">
-        <v>2164029972.832001</v>
+        <v>2095495467.56</v>
       </c>
       <c r="D3">
-        <v>12262836495.54799</v>
+        <v>11874474299.59</v>
       </c>
       <c r="E3">
-        <v>14426866468.38</v>
+        <v>13969969767.15</v>
       </c>
       <c r="F3">
-        <v>18141016054.17501</v>
+        <v>17634714703.94</v>
       </c>
       <c r="G3">
-        <v>15419863644.6</v>
+        <v>14989507496.93</v>
       </c>
       <c r="H3">
-        <v>1214990566.324999</v>
+        <v>1139045363.76</v>
       </c>
       <c r="I3">
         <v>1506161843.25</v>
       </c>
       <c r="J3">
-        <v>857060671.112</v>
+        <v>788526165.84</v>
       </c>
       <c r="K3">
-        <v>13119897166.66</v>
+        <v>12663000465.43</v>
       </c>
       <c r="L3">
         <v>1306969301.72</v>
@@ -509,34 +509,34 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>10325672734.77294</v>
+        <v>10323278549.5448</v>
       </c>
       <c r="D4">
-        <v>8600351632.791672</v>
+        <v>8586738394.717028</v>
       </c>
       <c r="E4">
-        <v>18926024367.56461</v>
+        <v>18910016944.26183</v>
       </c>
       <c r="F4">
-        <v>29969480477.93806</v>
+        <v>29789212833.82301</v>
       </c>
       <c r="G4">
-        <v>13544412775.82199</v>
+        <v>13391085667.5507</v>
       </c>
       <c r="H4">
-        <v>4077768999.606116</v>
+        <v>4050922760.012311</v>
       </c>
       <c r="I4">
-        <v>12347298702.50999</v>
+        <v>12347204406.26</v>
       </c>
       <c r="J4">
-        <v>2379190913.782944</v>
+        <v>2376796728.554799</v>
       </c>
       <c r="K4">
-        <v>10979542546.57462</v>
+        <v>10963535123.27183</v>
       </c>
       <c r="L4">
-        <v>7946481820.989984</v>
+        <v>7946481820.99</v>
       </c>
     </row>
     <row r="5">
@@ -546,31 +546,31 @@
         </is>
       </c>
       <c r="C5">
-        <v>867409.6799999997</v>
+        <v>433704.8399999999</v>
       </c>
       <c r="D5">
-        <v>4915321.495</v>
+        <v>2457660.7475</v>
       </c>
       <c r="E5">
-        <v>5782731.175</v>
+        <v>2891365.5875</v>
       </c>
       <c r="F5">
-        <v>7677453.895</v>
+        <v>2895764.4475</v>
       </c>
       <c r="G5">
-        <v>6525835.81</v>
+        <v>2461399.78</v>
       </c>
       <c r="H5">
-        <v>1057321.835</v>
+        <v>434364.6675</v>
       </c>
       <c r="I5">
-        <v>94296.25</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>867409.6800000001</v>
+        <v>433704.84</v>
       </c>
       <c r="K5">
-        <v>5782731.175</v>
+        <v>2891365.5875</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -586,34 +586,34 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>6984509573.66</v>
+        <v>6981418187.888666</v>
       </c>
       <c r="D6">
-        <v>39578887560.88999</v>
+        <v>39561369709.86514</v>
       </c>
       <c r="E6">
-        <v>46563397134.55</v>
+        <v>46542787897.7538</v>
       </c>
       <c r="F6">
-        <v>72610408158.64999</v>
+        <v>72509301609.59196</v>
       </c>
       <c r="G6">
-        <v>61718846934.83001</v>
+        <v>61632906368.13071</v>
       </c>
       <c r="H6">
-        <v>10891561223.82</v>
+        <v>10876395241.46125</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>6984509573.66</v>
+        <v>6981418187.888666</v>
       </c>
       <c r="K6">
-        <v>46563397134.55</v>
+        <v>46542787897.7538</v>
       </c>
       <c r="L6">
-        <v>3.539025783538818e-08</v>
+        <v>-2.030283212661743e-07</v>
       </c>
     </row>
     <row r="7">
@@ -626,34 +626,34 @@
         <v>0.4</v>
       </c>
       <c r="C7">
-        <v>8537538286.45</v>
+        <v>8449409756.46699</v>
       </c>
       <c r="D7">
-        <v>47284634479.89001</v>
+        <v>46785239476.89042</v>
       </c>
       <c r="E7">
-        <v>55822172766.34</v>
+        <v>55234649233.35741</v>
       </c>
       <c r="F7">
-        <v>84425017480.41</v>
+        <v>83484737175.4998</v>
       </c>
       <c r="G7">
-        <v>70855967496.17</v>
+        <v>70056729236.9969</v>
       </c>
       <c r="H7">
-        <v>11117113227.81</v>
+        <v>10976071182.07291</v>
       </c>
       <c r="I7">
-        <v>2451936756.429999</v>
+        <v>2451936756.43</v>
       </c>
       <c r="J7">
-        <v>7919198806.73</v>
+        <v>7831070276.74699</v>
       </c>
       <c r="K7">
-        <v>55203833286.62</v>
+        <v>54616309753.63741</v>
       </c>
       <c r="L7">
-        <v>618339479.7200005</v>
+        <v>618339479.7200003</v>
       </c>
     </row>
     <row r="8">
@@ -684,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>712003308.2500001</v>
+        <v>712003308.25</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -706,34 +706,34 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>44807040511.7363</v>
+        <v>38302367911.9211</v>
       </c>
       <c r="D9">
-        <v>35343424253.78708</v>
+        <v>31745404063.65495</v>
       </c>
       <c r="E9">
-        <v>80150464765.52338</v>
+        <v>70047771975.57605</v>
       </c>
       <c r="F9">
-        <v>142287495967.4269</v>
+        <v>125991790230.5634</v>
       </c>
       <c r="G9">
-        <v>66851383166.09001</v>
+        <v>60331477127.82437</v>
       </c>
       <c r="H9">
-        <v>1254904890.6</v>
+        <v>1253846940.470587</v>
       </c>
       <c r="I9">
-        <v>74181207910.73694</v>
+        <v>64406466162.26843</v>
       </c>
       <c r="J9">
-        <v>356622884.0099999</v>
+        <v>356622884.0100001</v>
       </c>
       <c r="K9">
-        <v>35700047137.79708</v>
+        <v>32102026947.66494</v>
       </c>
       <c r="L9">
-        <v>44450417627.7263</v>
+        <v>37945745027.9111</v>
       </c>
     </row>
     <row r="10">
@@ -746,16 +746,16 @@
         <v>0.4</v>
       </c>
       <c r="C10">
-        <v>1299181050.889999</v>
+        <v>1299181050.89</v>
       </c>
       <c r="D10">
         <v>1057614714.97</v>
       </c>
       <c r="E10">
-        <v>2356795765.860001</v>
+        <v>2356795765.86</v>
       </c>
       <c r="F10">
-        <v>4430773073.110002</v>
+        <v>4430773073.11</v>
       </c>
       <c r="G10">
         <v>2005634862.33</v>
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>2425138210.779999</v>
+        <v>2425138210.78</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -773,7 +773,7 @@
         <v>1057614714.97</v>
       </c>
       <c r="L10">
-        <v>1299181050.889999</v>
+        <v>1299181050.89</v>
       </c>
     </row>
     <row r="11">
@@ -786,34 +786,34 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>14495148687.89369</v>
+        <v>14491894433.37137</v>
       </c>
       <c r="D11">
-        <v>10141235682.10291</v>
+        <v>10138046070.21396</v>
       </c>
       <c r="E11">
-        <v>24636384369.99663</v>
+        <v>24629940503.58532</v>
       </c>
       <c r="F11">
-        <v>56318703986.46306</v>
+        <v>56258741421.84528</v>
       </c>
       <c r="G11">
-        <v>22702852766.89995</v>
+        <v>22671481222.51871</v>
       </c>
       <c r="H11">
         <v>29969062.5</v>
       </c>
       <c r="I11">
-        <v>33585882157.06313</v>
+        <v>33557291136.82656</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>10141235682.10291</v>
+        <v>10138046070.21396</v>
       </c>
       <c r="L11">
-        <v>14495148687.89369</v>
+        <v>14491894433.37137</v>
       </c>
     </row>
     <row r="12">
@@ -863,34 +863,34 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>2304709424.4</v>
+        <v>2233600213.363579</v>
       </c>
       <c r="D13">
-        <v>2304679415.55</v>
+        <v>2233570204.555042</v>
       </c>
       <c r="E13">
-        <v>4609388839.950001</v>
+        <v>4467170417.918622</v>
       </c>
       <c r="F13">
-        <v>7288225897.830001</v>
+        <v>7008425150.000095</v>
       </c>
       <c r="G13">
-        <v>3644112948.11</v>
+        <v>3504212574.197531</v>
       </c>
       <c r="H13">
-        <v>3048571137.28</v>
+        <v>2945860175.324294</v>
       </c>
       <c r="I13">
-        <v>595541812.4400001</v>
+        <v>558352400.4782691</v>
       </c>
       <c r="J13">
-        <v>1930259534.09</v>
+        <v>1868029778.248265</v>
       </c>
       <c r="K13">
-        <v>4234938949.640001</v>
+        <v>4101599982.803307</v>
       </c>
       <c r="L13">
-        <v>374449890.3099999</v>
+        <v>365570435.1153149</v>
       </c>
     </row>
     <row r="14">
@@ -955,7 +955,7 @@
         <v>1793407125.88</v>
       </c>
       <c r="G15">
-        <v>896703562.8999999</v>
+        <v>896703562.9</v>
       </c>
       <c r="H15">
         <v>660463502.37</v>
@@ -967,10 +967,10 @@
         <v>366695683.76</v>
       </c>
       <c r="K15">
-        <v>873986284.6800001</v>
+        <v>873986284.6799999</v>
       </c>
       <c r="L15">
-        <v>140594917.4299999</v>
+        <v>140594917.43</v>
       </c>
     </row>
     <row r="16">
@@ -983,34 +983,34 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>789163859.0899999</v>
+        <v>786725549.6023514</v>
       </c>
       <c r="D16">
-        <v>4471928503.59</v>
+        <v>4458111417.312308</v>
       </c>
       <c r="E16">
-        <v>5261092362.679998</v>
+        <v>5244836966.91466</v>
       </c>
       <c r="F16">
-        <v>7288823769.32</v>
+        <v>7185129211.911049</v>
       </c>
       <c r="G16">
-        <v>6195500203.380001</v>
+        <v>6107359829.589524</v>
       </c>
       <c r="H16">
-        <v>1093323565.94</v>
+        <v>1077769382.321525</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>789163859.0899998</v>
+        <v>786725549.6023514</v>
       </c>
       <c r="K16">
-        <v>5261092362.679998</v>
+        <v>5244836966.91466</v>
       </c>
       <c r="L16">
-        <v>3.748573362827301e-08</v>
+        <v>2.621673047513547e-08</v>
       </c>
     </row>
     <row r="17">
@@ -1029,13 +1029,13 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>6172500</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>5246625</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>925875</v>
+        <v>0</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1060,34 +1060,34 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>12705986793.09833</v>
+        <v>11723490376.01386</v>
       </c>
       <c r="D18">
-        <v>53497453280.98832</v>
+        <v>48783070057.32639</v>
       </c>
       <c r="E18">
-        <v>66203440074.08664</v>
+        <v>60506560433.34026</v>
       </c>
       <c r="F18">
-        <v>97048528771.97334</v>
+        <v>88064258036.46448</v>
       </c>
       <c r="G18">
-        <v>78221343744.46829</v>
+        <v>70797148996.39685</v>
       </c>
       <c r="H18">
-        <v>17011585211.285</v>
+        <v>15564019928.70356</v>
       </c>
       <c r="I18">
-        <v>1815599816.22</v>
+        <v>1703089111.364068</v>
       </c>
       <c r="J18">
-        <v>11252376336.65833</v>
+        <v>10362905044.20415</v>
       </c>
       <c r="K18">
-        <v>64749829617.64666</v>
+        <v>59145975101.53053</v>
       </c>
       <c r="L18">
-        <v>1453610456.439999</v>
+        <v>1360585331.809717</v>
       </c>
     </row>
     <row r="19">
@@ -1097,31 +1097,31 @@
         </is>
       </c>
       <c r="C19">
-        <v>29476.58166666665</v>
+        <v>4439.488935185183</v>
       </c>
       <c r="D19">
-        <v>136940.7516666667</v>
+        <v>17633.82587962963</v>
       </c>
       <c r="E19">
-        <v>166417.3333333333</v>
+        <v>22073.31481481481</v>
       </c>
       <c r="F19">
-        <v>260153528.1066667</v>
+        <v>28000617.61833333</v>
       </c>
       <c r="G19">
-        <v>174334321.2016667</v>
+        <v>18622528.01861111</v>
       </c>
       <c r="H19">
-        <v>85819206.90500002</v>
+        <v>9378089.599722221</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19">
-        <v>29476.58166666667</v>
+        <v>4439.488935185185</v>
       </c>
       <c r="K19">
-        <v>166417.3333333333</v>
+        <v>22073.31481481481</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -1137,34 +1137,34 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>9810661336.040005</v>
+        <v>9052732403.779791</v>
       </c>
       <c r="D20">
-        <v>46471547949.11</v>
+        <v>42744683996.36911</v>
       </c>
       <c r="E20">
-        <v>56282209285.15</v>
+        <v>51797416400.1489</v>
       </c>
       <c r="F20">
-        <v>82041892473.20001</v>
+        <v>73449196423.68405</v>
       </c>
       <c r="G20">
-        <v>67502789465.26502</v>
+        <v>60423967776.9254</v>
       </c>
       <c r="H20">
-        <v>13469196922.27502</v>
+        <v>12165030111.56466</v>
       </c>
       <c r="I20">
-        <v>1069906085.659999</v>
+        <v>860198535.1939973</v>
       </c>
       <c r="J20">
-        <v>9133423181.320005</v>
+        <v>8500745193.308492</v>
       </c>
       <c r="K20">
-        <v>55604971130.43</v>
+        <v>51245429189.6776</v>
       </c>
       <c r="L20">
-        <v>677238154.7200003</v>
+        <v>551987210.4712989</v>
       </c>
     </row>
     <row r="21">
@@ -1183,13 +1183,13 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>1252357157.5</v>
+        <v>313089289.375</v>
       </c>
       <c r="G21">
-        <v>1008422224.775</v>
+        <v>252105556.19375</v>
       </c>
       <c r="H21">
-        <v>243934932.725</v>
+        <v>60983733.18125</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1214,34 +1214,34 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>4527541390.320003</v>
+        <v>5405662882.735476</v>
       </c>
       <c r="D22">
-        <v>21939499670.81</v>
+        <v>25345869977.45417</v>
       </c>
       <c r="E22">
-        <v>26467041061.13</v>
+        <v>30751532860.18965</v>
       </c>
       <c r="F22">
-        <v>32836502055.67001</v>
+        <v>39312408397.66499</v>
       </c>
       <c r="G22">
-        <v>26473257804.31001</v>
+        <v>31701535546.70824</v>
       </c>
       <c r="H22">
-        <v>4492958947.18</v>
+        <v>5435053992.325138</v>
       </c>
       <c r="I22">
-        <v>1870285304.18</v>
+        <v>2175818858.631612</v>
       </c>
       <c r="J22">
-        <v>3680484616.850002</v>
+        <v>4431004403.013864</v>
       </c>
       <c r="K22">
-        <v>25619984287.66</v>
+        <v>29776874380.46804</v>
       </c>
       <c r="L22">
-        <v>847056773.4700004</v>
+        <v>974658479.721612</v>
       </c>
     </row>
     <row r="23">
@@ -1254,34 +1254,34 @@
         <v>0.4</v>
       </c>
       <c r="C23">
-        <v>3435614356.359999</v>
+        <v>2551355021.62</v>
       </c>
       <c r="D23">
-        <v>20927127152.56</v>
+        <v>17502658082.76</v>
       </c>
       <c r="E23">
-        <v>24362741508.92</v>
+        <v>20054013104.38</v>
       </c>
       <c r="F23">
-        <v>35351042552.18999</v>
+        <v>28793401667.05</v>
       </c>
       <c r="G23">
-        <v>29858601322.59</v>
+        <v>24584486245.37</v>
       </c>
       <c r="H23">
-        <v>1965065904.88</v>
+        <v>1022459827.08</v>
       </c>
       <c r="I23">
-        <v>3527375324.72</v>
+        <v>3186455594.6</v>
       </c>
       <c r="J23">
-        <v>1365954139.929999</v>
+        <v>614924230.86</v>
       </c>
       <c r="K23">
-        <v>22293081292.49</v>
+        <v>18117582313.62</v>
       </c>
       <c r="L23">
-        <v>2069660216.43</v>
+        <v>1936430790.76</v>
       </c>
     </row>
     <row r="24">
@@ -1294,34 +1294,34 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>7913285650.129994</v>
+        <v>7913285650.13</v>
       </c>
       <c r="D24">
-        <v>6364840433.529999</v>
+        <v>6364840433.53</v>
       </c>
       <c r="E24">
-        <v>14278126083.65998</v>
+        <v>14278126083.66</v>
       </c>
       <c r="F24">
-        <v>22774859324.27998</v>
+        <v>22774859324.28</v>
       </c>
       <c r="G24">
         <v>10052330928.07</v>
       </c>
       <c r="H24">
-        <v>12549681010.48001</v>
+        <v>12549681010.48</v>
       </c>
       <c r="I24">
         <v>172847385.73</v>
       </c>
       <c r="J24">
-        <v>7856238536.949991</v>
+        <v>7856238536.95</v>
       </c>
       <c r="K24">
-        <v>14221078970.47998</v>
+        <v>14221078970.48</v>
       </c>
       <c r="L24">
-        <v>57047113.17999998</v>
+        <v>57047113.17999994</v>
       </c>
     </row>
     <row r="25">

</xml_diff>